<commit_message>
corrected rna date on s1 10.01.20
</commit_message>
<xml_diff>
--- a/rnaSample/rnaSample_H.BROWN_09.04.20.xlsx
+++ b/rnaSample/rnaSample_H.BROWN_09.04.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/rnaSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377CCE0E-6FA1-3141-8E78-B781D48ED6A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A346E0-3B18-5A40-82B2-1DB7B01FD114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6460" yWindow="460" windowWidth="22720" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD50"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>